<commit_message>
AI words to 30
</commit_message>
<xml_diff>
--- a/AI-words.xlsx
+++ b/AI-words.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Eng</t>
   </si>
@@ -42,15 +42,9 @@
     <t>ear</t>
   </si>
   <si>
-    <t>tai</t>
-  </si>
-  <si>
     <t>hand</t>
   </si>
   <si>
-    <t>tay</t>
-  </si>
-  <si>
     <t>bed</t>
   </si>
   <si>
@@ -72,24 +66,156 @@
     <t>elephant</t>
   </si>
   <si>
-    <t>voi</t>
-  </si>
-  <si>
     <t>pandar</t>
   </si>
   <si>
-    <t>báo</t>
+    <t>tiger</t>
+  </si>
+  <si>
+    <t>cat</t>
+  </si>
+  <si>
+    <t>machine</t>
+  </si>
+  <si>
+    <t>máy</t>
+  </si>
+  <si>
+    <t>ant</t>
+  </si>
+  <si>
+    <t>con kiến</t>
+  </si>
+  <si>
+    <t>alibi</t>
+  </si>
+  <si>
+    <t>bằng chứng</t>
+  </si>
+  <si>
+    <t>epidemic</t>
+  </si>
+  <si>
+    <t>aroma</t>
+  </si>
+  <si>
+    <t>book</t>
+  </si>
+  <si>
+    <t>happy</t>
+  </si>
+  <si>
+    <t>asthetic</t>
+  </si>
+  <si>
+    <t>computer</t>
+  </si>
+  <si>
+    <t>máy vi tính</t>
+  </si>
+  <si>
+    <t>con mèo</t>
+  </si>
+  <si>
+    <t>con hổ</t>
+  </si>
+  <si>
+    <t>con báo</t>
+  </si>
+  <si>
+    <t>con voi</t>
+  </si>
+  <si>
+    <t>thẩm mỹ</t>
+  </si>
+  <si>
+    <t>hạnh phúc</t>
+  </si>
+  <si>
+    <t>cuốn sách</t>
+  </si>
+  <si>
+    <t>hương thơm</t>
+  </si>
+  <si>
+    <t>nurse</t>
+  </si>
+  <si>
+    <t>ý tá</t>
+  </si>
+  <si>
+    <t>dịch bệnh</t>
+  </si>
+  <si>
+    <t>hospital</t>
+  </si>
+  <si>
+    <t>bệnh viện</t>
+  </si>
+  <si>
+    <t>bàn tay</t>
+  </si>
+  <si>
+    <t>run</t>
+  </si>
+  <si>
+    <t>chạy</t>
+  </si>
+  <si>
+    <t>kiss</t>
+  </si>
+  <si>
+    <t>hôn</t>
+  </si>
+  <si>
+    <t>lỗ tai</t>
+  </si>
+  <si>
+    <t>jump</t>
+  </si>
+  <si>
+    <t>nhảy</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>bình luận</t>
+  </si>
+  <si>
+    <t>horror</t>
+  </si>
+  <si>
+    <t>kinh dị</t>
+  </si>
+  <si>
+    <t>cinema</t>
+  </si>
+  <si>
+    <t>rạp phim</t>
+  </si>
+  <si>
+    <t>office</t>
+  </si>
+  <si>
+    <t>văn phòng</t>
+  </si>
+  <si>
+    <t>formular</t>
+  </si>
+  <si>
+    <t>công thức</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -388,7 +514,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -396,13 +522,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -414,74 +543,242 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B14" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add: anagram ai words
</commit_message>
<xml_diff>
--- a/AI-words.xlsx
+++ b/AI-words.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>Eng</t>
   </si>
@@ -201,10 +201,28 @@
     <t>văn phòng</t>
   </si>
   <si>
-    <t>formular</t>
-  </si>
-  <si>
     <t>công thức</t>
+  </si>
+  <si>
+    <t>formula</t>
+  </si>
+  <si>
+    <t>meat</t>
+  </si>
+  <si>
+    <t>thịt</t>
+  </si>
+  <si>
+    <t>team</t>
+  </si>
+  <si>
+    <t>nhóm</t>
+  </si>
+  <si>
+    <t>mate</t>
+  </si>
+  <si>
+    <t>bạn</t>
   </si>
 </sst>
 </file>
@@ -514,7 +532,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -522,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,10 +793,34 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" t="s">
         <v>60</v>
       </c>
-      <c r="B31" t="s">
-        <v>61</v>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated: 50 words AI dataset
</commit_message>
<xml_diff>
--- a/AI-words.xlsx
+++ b/AI-words.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
-  <si>
-    <t>Eng</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t>VN</t>
   </si>
@@ -223,17 +220,122 @@
   </si>
   <si>
     <t>bạn</t>
+  </si>
+  <si>
+    <t>apartment</t>
+  </si>
+  <si>
+    <t>căn hộ</t>
+  </si>
+  <si>
+    <t>document</t>
+  </si>
+  <si>
+    <t>tài liệu</t>
+  </si>
+  <si>
+    <t>electricity</t>
+  </si>
+  <si>
+    <t>điện</t>
+  </si>
+  <si>
+    <t>ENG</t>
+  </si>
+  <si>
+    <t>jar</t>
+  </si>
+  <si>
+    <t>cái lọ</t>
+  </si>
+  <si>
+    <t>purse</t>
+  </si>
+  <si>
+    <t>cái ví</t>
+  </si>
+  <si>
+    <t>strength</t>
+  </si>
+  <si>
+    <t>sức mạnh</t>
+  </si>
+  <si>
+    <t>vegetable</t>
+  </si>
+  <si>
+    <t>rau củ</t>
+  </si>
+  <si>
+    <t>mathematician</t>
+  </si>
+  <si>
+    <t>nhà toán học</t>
+  </si>
+  <si>
+    <t>physicist</t>
+  </si>
+  <si>
+    <t>nhà vật lý</t>
+  </si>
+  <si>
+    <t>scientist</t>
+  </si>
+  <si>
+    <t>nhà khoa học</t>
+  </si>
+  <si>
+    <t>circuit</t>
+  </si>
+  <si>
+    <t>bo mạch</t>
+  </si>
+  <si>
+    <t>napkin</t>
+  </si>
+  <si>
+    <t>khăn ăn</t>
+  </si>
+  <si>
+    <t>construction</t>
+  </si>
+  <si>
+    <t>công trường</t>
+  </si>
+  <si>
+    <t>saucepan</t>
+  </si>
+  <si>
+    <t>cái chảo</t>
+  </si>
+  <si>
+    <t>cupboard</t>
+  </si>
+  <si>
+    <t>tủ đựng chén</t>
+  </si>
+  <si>
+    <t>chopsticks</t>
+  </si>
+  <si>
+    <t>đôi đũa</t>
+  </si>
+  <si>
+    <t>spoon</t>
+  </si>
+  <si>
+    <t>cái muỗng</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -532,7 +634,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -540,180 +642,181 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
         <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
         <v>35</v>
@@ -721,109 +824,248 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" t="s">
         <v>42</v>
-      </c>
-      <c r="B23" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
         <v>47</v>
-      </c>
-      <c r="B25" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" t="s">
         <v>58</v>
-      </c>
-      <c r="B30" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>63</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:B37">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>